<commit_message>
Mon Dec  5 15:32:03 RTZ 2022
</commit_message>
<xml_diff>
--- a/то_чем_я_никогда_больше_не_буду_заниматься_в_этой_жизни/Отчет №3.xlsx
+++ b/то_чем_я_никогда_больше_не_буду_заниматься_в_этой_жизни/Отчет №3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Desktop\3sem\то_чем_я_никогда_больше_не_буду_заниматься_в_этой_жизни\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{130319C0-7827-43B2-95D8-91555C1E6D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35489F3C-E96A-433A-9E4D-2F3779216FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{74E68520-AA6B-4EAE-AFDD-D8A3B359A190}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -96,8 +96,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -199,6 +199,9 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>Физ.нагрузка (Ккал)</c:v>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent3"/>
@@ -308,6 +311,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Кол-во Ккал в день</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -460,6 +466,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Вес(кг)</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -766,6 +775,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="958779280"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
@@ -1737,7 +1747,7 @@
   <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E16"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>